<commit_message>
excel with measurements for building 1 updated
</commit_message>
<xml_diff>
--- a/doc/Sprint_1/1231267/Measurements_Building1.xlsx
+++ b/doc/Sprint_1/1231267/Measurements_Building1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270EF668-953D-4EB6-8B9D-7AC80E3B31D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035ED6AE-9CA5-45CA-960A-D5648B9CF9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Cable Measurements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
   <si>
     <t>Rooms</t>
   </si>
@@ -419,15 +419,6 @@
   </si>
   <si>
     <t>Length of Material Needed For Outside</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance from Buulding 1 </t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -546,13 +537,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -903,7 +891,7 @@
   <dimension ref="B1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,87 +904,87 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="S2" s="4" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
     </row>
     <row r="3" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1">
         <v>744.43</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3">
         <v>429.31</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="M3" s="4" t="s">
+      <c r="J3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3">
         <v>315.12</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="S3" s="4" t="s">
+      <c r="P3" s="3"/>
+      <c r="S3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4">
+      <c r="T3" s="3"/>
+      <c r="U3" s="3">
         <v>2.5</v>
       </c>
-      <c r="V3" s="4"/>
+      <c r="V3" s="3"/>
     </row>
     <row r="4" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1">
-        <v>614</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>15.5</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="M4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="M4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4">
-        <v>6</v>
-      </c>
-      <c r="P4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1010,12 +998,12 @@
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
@@ -1033,16 +1021,10 @@
       <c r="H10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="Q10" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>128</v>
-      </c>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
@@ -1060,16 +1042,10 @@
       <c r="H11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>35.5</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="Q11" s="1">
-        <v>2</v>
-      </c>
-      <c r="R11" s="1">
-        <v>81.5</v>
-      </c>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
@@ -1087,16 +1063,10 @@
       <c r="H12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>26</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="Q12" s="1">
-        <v>3</v>
-      </c>
-      <c r="R12" s="1">
-        <v>290</v>
-      </c>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
@@ -1109,13 +1079,7 @@
         <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>4</v>
-      </c>
-      <c r="R13" s="1">
-        <v>234</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1128,13 +1092,6 @@
       <c r="D14" s="1">
         <v>10</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="R14" s="1">
-        <f>SUM(R11:R13)</f>
-        <v>605.5</v>
-      </c>
     </row>
     <row r="15" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
@@ -1219,8 +1176,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <f>SUM(D10:D21)</f>
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1214,7 @@
   <dimension ref="B2:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,334 +1226,334 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="I3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="F4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>7.5</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="F5" s="3"/>
+      <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="I6" s="4" t="s">
+      <c r="F6" s="3"/>
+      <c r="I6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5" t="s">
+      <c r="J6" s="3"/>
+      <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="5" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-      <c r="I9" s="4" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="I9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="5" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="1">
         <v>15</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="5" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="1">
         <v>7.75</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5" t="s">
+      <c r="J11" s="3"/>
+      <c r="K11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1">
         <v>1.5</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="5" t="s">
+      <c r="J12" s="3"/>
+      <c r="K12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="1">
         <v>10.5</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="3"/>
+      <c r="K13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="1">
         <v>18</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="5" t="s">
+      <c r="J14" s="3"/>
+      <c r="K14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="1">
         <f>SUM(G10:G14)</f>
         <v>52.75</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="5" t="s">
+      <c r="J15" s="3"/>
+      <c r="K15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="1">
         <v>24.5</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="1">
         <v>7.5</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="1">
         <f>SUM(G21:G24)</f>
         <v>64</v>
@@ -1605,10 +1561,10 @@
     </row>
     <row r="26" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="1">
         <v>116.75</v>
       </c>
@@ -1646,6 +1602,8 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I7:J7"/>
@@ -1662,8 +1620,6 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L14"/>
@@ -1729,926 +1685,926 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="I6" s="4" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="I6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3">
         <f>SUM(D7:F54)</f>
         <v>341.05999999999989</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <v>10.43</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="I7" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3">
         <f>SUM(D56:F86)</f>
         <v>225.11999999999998</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
         <v>12.03</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="I8" s="4" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="I8" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
         <f>SUM(K6:M7)</f>
         <v>566.17999999999984</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>7.57</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <v>9.17</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
         <v>7.03</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
         <v>8.6300000000000008</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <v>5.6</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
         <v>10.79</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
         <v>12.39</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
         <v>7.93</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
         <v>9.5299999999999994</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
         <v>7.39</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
         <v>8.99</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
         <v>4</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
         <v>5.6</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
         <v>11.99</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
         <v>10.14</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
         <v>6.81</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5">
+      <c r="C30" s="5"/>
+      <c r="D30" s="4">
         <v>5.34</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4">
         <v>3.87</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5">
+      <c r="C32" s="5"/>
+      <c r="D32" s="4">
         <v>5.96</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="5">
+      <c r="C33" s="5"/>
+      <c r="D33" s="4">
         <v>7.75</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="5">
+      <c r="C34" s="5"/>
+      <c r="D34" s="4">
         <v>11.01</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="5">
+      <c r="C35" s="5"/>
+      <c r="D35" s="4">
         <v>12.48</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3">
         <v>13.95</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
         <v>10.78</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3">
         <v>8.82</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
         <v>5.38</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5">
+      <c r="C41" s="5"/>
+      <c r="D41" s="4">
         <v>3.89</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5">
+      <c r="C43" s="5"/>
+      <c r="D43" s="4">
         <v>6.32</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
         <v>13.46</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3">
         <v>11.5</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3">
         <v>8.1199999999999992</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
         <v>6.69</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="5">
+      <c r="C49" s="5"/>
+      <c r="D49" s="4">
         <v>5.26</v>
       </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="5">
+      <c r="C50" s="5"/>
+      <c r="D50" s="4">
         <v>3.83</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="5">
+      <c r="C51" s="5"/>
+      <c r="D51" s="4">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="5">
+      <c r="C52" s="5"/>
+      <c r="D52" s="4">
         <v>6.32</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="5">
+      <c r="C53" s="5"/>
+      <c r="D53" s="4">
         <v>9.9600000000000009</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="5"/>
     </row>
     <row r="54" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="5">
+      <c r="C54" s="5"/>
+      <c r="D54" s="4">
         <v>11.63</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="F54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3">
         <v>4.3899999999999997</v>
       </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3">
         <v>6.18</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3">
         <v>7.97</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
     </row>
     <row r="59" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3">
         <v>7.96</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="5">
+      <c r="C60" s="5"/>
+      <c r="D60" s="4">
         <v>9.75</v>
       </c>
-      <c r="E60" s="7"/>
-      <c r="F60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="5"/>
     </row>
     <row r="61" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="5">
+      <c r="C61" s="5"/>
+      <c r="D61" s="4">
         <v>11.54</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4" t="s">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
     </row>
     <row r="63" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3">
         <v>7.96</v>
       </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3">
         <v>9.75</v>
       </c>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
     </row>
     <row r="65" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3">
         <v>11.54</v>
       </c>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
     </row>
     <row r="66" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3">
         <v>4.3899999999999997</v>
       </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
     </row>
     <row r="67" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="5">
+      <c r="C67" s="5"/>
+      <c r="D67" s="4">
         <v>6.18</v>
       </c>
-      <c r="E67" s="7"/>
-      <c r="F67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="5">
+      <c r="C68" s="5"/>
+      <c r="D68" s="4">
         <v>7.97</v>
       </c>
-      <c r="E68" s="7"/>
-      <c r="F68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
     </row>
     <row r="70" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3">
         <v>10.98</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
     </row>
     <row r="71" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3">
         <v>9.02</v>
       </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
     </row>
     <row r="72" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3">
         <v>5.58</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
     </row>
     <row r="73" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3">
         <v>4.09</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
     </row>
     <row r="74" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="5">
+      <c r="C74" s="5"/>
+      <c r="D74" s="4">
         <v>4.5599999999999996</v>
       </c>
-      <c r="E74" s="7"/>
-      <c r="F74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="5">
+      <c r="C75" s="5"/>
+      <c r="D75" s="4">
         <v>6.52</v>
       </c>
-      <c r="E75" s="7"/>
-      <c r="F75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
     </row>
     <row r="77" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3">
         <v>13.66</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
     </row>
     <row r="78" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3">
         <v>11.7</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
     </row>
     <row r="79" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3">
         <v>7.97</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
     </row>
     <row r="80" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3">
         <v>6.18</v>
       </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
     </row>
     <row r="81" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3">
         <v>4.3899999999999997</v>
       </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
     </row>
     <row r="82" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3">
         <v>4.5599999999999996</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
     </row>
     <row r="83" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3">
         <v>6.52</v>
       </c>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
     </row>
     <row r="84" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3">
         <v>9.8800000000000008</v>
       </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
     </row>
     <row r="85" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3">
         <v>11.27</v>
       </c>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
     </row>
     <row r="86" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3">
         <v>12.66</v>
       </c>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
     </row>
     <row r="87" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -2701,12 +2657,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D26:F26"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
@@ -2716,28 +2666,29 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D26:F26"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D37:F37"/>
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="D33:F33"/>
     <mergeCell ref="D34:F34"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D37:F37"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B36:C36"/>
@@ -2747,6 +2698,11 @@
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B49:C49"/>

</xml_diff>